<commit_message>
Beezon in the trap
Completed
</commit_message>
<xml_diff>
--- a/OverworldRouting.xlsx
+++ b/OverworldRouting.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="202">
   <si>
     <t>Proposed Overworld Route</t>
   </si>
@@ -75,12 +75,6 @@
     <t>Get cape here, it’s a significant detour, but saves lots of time.</t>
   </si>
   <si>
-    <t>Yoshi's House</t>
-  </si>
-  <si>
-    <t>Get overworld boot</t>
-  </si>
-  <si>
     <t>Mushroom Ledge B</t>
   </si>
   <si>
@@ -157,9 +151,6 @@
 also we can pretty much ignore yoshi, as the dragon coin glitch takes us to a slow level, and only has 2 dragon coins. Perhaps may save time in some very long levels. There are some glitches involving the halfway gate when using yoshi wings, which can take you to alternate levels.</t>
   </si>
   <si>
-    <t>Get the first 1</t>
-  </si>
-  <si>
     <t>Just fly under it</t>
   </si>
   <si>
@@ -199,9 +190,6 @@
     <t>This Cavern is dumb</t>
   </si>
   <si>
-    <t>Level 91 in Lunar Magic, fly under the level so you don't have to wait for the jocks</t>
-  </si>
-  <si>
     <t>Autoscroll</t>
   </si>
   <si>
@@ -215,9 +203,6 @@
   </si>
   <si>
     <t>Tunnel of the Living Rock</t>
-  </si>
-  <si>
-    <t>Leave Koume's fortress to the end, as you'll lose your powerup</t>
   </si>
   <si>
     <t>The Dumbest cavern A</t>
@@ -265,9 +250,6 @@
     <t>Most Likely</t>
   </si>
   <si>
-    <t>Maybe possible to fly from the second to the third dragon coin above the level.</t>
-  </si>
-  <si>
     <t>Melt a Meat locker!</t>
   </si>
   <si>
@@ -392,6 +374,270 @@
   </si>
   <si>
     <t>Luminous Leapings B</t>
+  </si>
+  <si>
+    <t>Keep a Positive Altitude</t>
+  </si>
+  <si>
+    <t>Cryophobia Cavern</t>
+  </si>
+  <si>
+    <t>Gourmet Hindrance</t>
+  </si>
+  <si>
+    <t>Baseball Mountain</t>
+  </si>
+  <si>
+    <t>Disco Dance Party</t>
+  </si>
+  <si>
+    <t>Chains of atrophy (b)</t>
+  </si>
+  <si>
+    <t>Pixel perfect</t>
+  </si>
+  <si>
+    <t>Luminous leapings A</t>
+  </si>
+  <si>
+    <t>Polished pipeline A</t>
+  </si>
+  <si>
+    <t>Manky bridge</t>
+  </si>
+  <si>
+    <t>Mushroom tripper</t>
+  </si>
+  <si>
+    <t>The Smog that Smiles back</t>
+  </si>
+  <si>
+    <t>Polished Pipeline B</t>
+  </si>
+  <si>
+    <t>Maybe swap polished pipeline exits depending on speed of overworld</t>
+  </si>
+  <si>
+    <t>Disarray</t>
+  </si>
+  <si>
+    <t>Slower</t>
+  </si>
+  <si>
+    <t>Chains of atrophy (a)</t>
+  </si>
+  <si>
+    <t>Do both luminous leapings exits here while you still have the cape</t>
+  </si>
+  <si>
+    <t>Do both chains of atrophy exits while you still have cape</t>
+  </si>
+  <si>
+    <t>Wigglertuff</t>
+  </si>
+  <si>
+    <t>The Ruins of Challenging sadness</t>
+  </si>
+  <si>
+    <t>Coin Guides are Always Accurate! B</t>
+  </si>
+  <si>
+    <t>Coin Guides are Always Accurate! A</t>
+  </si>
+  <si>
+    <t>Into The Dark forest B</t>
+  </si>
+  <si>
+    <t>Into The dark forest A</t>
+  </si>
+  <si>
+    <t>House of Holy B</t>
+  </si>
+  <si>
+    <t>All the Way from New Jersey</t>
+  </si>
+  <si>
+    <t>Get the Secret Exit B</t>
+  </si>
+  <si>
+    <t>Get the Secret Exit A</t>
+  </si>
+  <si>
+    <t>Shouldering On</t>
+  </si>
+  <si>
+    <t>Old Fogey Skie</t>
+  </si>
+  <si>
+    <t>The Green Switch</t>
+  </si>
+  <si>
+    <t>House of Holy A</t>
+  </si>
+  <si>
+    <t>BALLS!</t>
+  </si>
+  <si>
+    <t>The Trees Are Dead</t>
+  </si>
+  <si>
+    <t>Get cape here. Maybe you can duplicate the turn block and get a key from the last dragon coin to enter the door early.</t>
+  </si>
+  <si>
+    <t>Shell Shrine</t>
+  </si>
+  <si>
+    <t>Lose cape</t>
+  </si>
+  <si>
+    <t>Gain cape</t>
+  </si>
+  <si>
+    <t>Maybe do this after bowser? Maybe with yoshi?</t>
+  </si>
+  <si>
+    <t>Lose cape/Gain cape</t>
+  </si>
+  <si>
+    <t>The Lava gap B</t>
+  </si>
+  <si>
+    <t>Think Fast!</t>
+  </si>
+  <si>
+    <t>Rock Climbing Rush</t>
+  </si>
+  <si>
+    <t>The Lava Gap A</t>
+  </si>
+  <si>
+    <t>Burnt mountain Tango</t>
+  </si>
+  <si>
+    <t>Industrial interior</t>
+  </si>
+  <si>
+    <t>Skulliloquy</t>
+  </si>
+  <si>
+    <t>We Haven't had enough thwomps A</t>
+  </si>
+  <si>
+    <t>Root of Yggdrasil</t>
+  </si>
+  <si>
+    <t>Scaffolding Scuffle</t>
+  </si>
+  <si>
+    <t>Ludwig's grindhouse</t>
+  </si>
+  <si>
+    <t>Return here to get cape for next level</t>
+  </si>
+  <si>
+    <t>Normal exit first, then return to get last dragon coin, then start select out of level</t>
+  </si>
+  <si>
+    <t>We Haven't had enough thwomps B</t>
+  </si>
+  <si>
+    <t>Impetuous Athletic</t>
+  </si>
+  <si>
+    <t>Maybe do pixel perfect after here if yoshi does not take too long to get.</t>
+  </si>
+  <si>
+    <t>Suspicious Warehouse</t>
+  </si>
+  <si>
+    <t>Aquiferic pressure A</t>
+  </si>
+  <si>
+    <t>Rupture of the deep B</t>
+  </si>
+  <si>
+    <t>Rupture of the deep A</t>
+  </si>
+  <si>
+    <t>Fortress of Koumei's Trap</t>
+  </si>
+  <si>
+    <t>Aquiferic Pressure B</t>
+  </si>
+  <si>
+    <t>Back to the Future!</t>
+  </si>
+  <si>
+    <t>Tactical Ambush operation</t>
+  </si>
+  <si>
+    <t>Super Ultra Grand Marathon on Finalness</t>
+  </si>
+  <si>
+    <t>The Black Hole</t>
+  </si>
+  <si>
+    <t>Miscelaneous Monument</t>
+  </si>
+  <si>
+    <t>The Depraved Stronghold</t>
+  </si>
+  <si>
+    <t>Shattered Dreams</t>
+  </si>
+  <si>
+    <t>Aquiferic Pressure A</t>
+  </si>
+  <si>
+    <t>Get overwold boot</t>
+  </si>
+  <si>
+    <t>Shell Sticker</t>
+  </si>
+  <si>
+    <t>1F8</t>
+  </si>
+  <si>
+    <t>Bowser's Castle</t>
+  </si>
+  <si>
+    <t>Roy's terrible Sadistic Castle A</t>
+  </si>
+  <si>
+    <t>Siberian Precipice A</t>
+  </si>
+  <si>
+    <t>PEEK-A-BOO A</t>
+  </si>
+  <si>
+    <t>Get the first 2</t>
+  </si>
+  <si>
+    <t>Pretty limited route options here.</t>
+  </si>
+  <si>
+    <t>No yoshi</t>
+  </si>
+  <si>
+    <t>No Yoshi</t>
+  </si>
+  <si>
+    <t>Possibility of sequnce breaks using the yoshi</t>
+  </si>
+  <si>
+    <t>Maybe possible to fly from the second to the third dragon coin above the level. Consider dragon coin glitch? Do level after cool kickin?</t>
+  </si>
+  <si>
+    <t>Leave Koumei's fortress to the end, as you'll lose your powerup</t>
+  </si>
+  <si>
+    <t>Level 90 in Lunar Magic, fly under the level so you don't have to wait for the jocks Dragon coin glitch possibility here</t>
+  </si>
+  <si>
+    <t>Try it!</t>
+  </si>
+  <si>
+    <t>Maybe try flying in the first part of this level Maybe also keep yoshi</t>
   </si>
 </sst>
 </file>
@@ -467,18 +713,6 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -496,6 +730,18 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -789,17 +1035,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I167"/>
+  <dimension ref="A1:I172"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F64" sqref="F64"/>
+      <pane ySplit="2" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I68" sqref="I68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="42.42578125" customWidth="1"/>
     <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" customWidth="1"/>
     <col min="9" max="9" width="61.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -828,7 +1075,7 @@
         <v>7</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>8</v>
@@ -886,7 +1133,7 @@
         <v>13</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -964,29 +1211,41 @@
       <c r="H7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="5"/>
+      <c r="I7" s="4" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="H8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" ht="30">
       <c r="A9" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>9</v>
@@ -995,7 +1254,7 @@
         <v>9</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>10</v>
@@ -1006,43 +1265,47 @@
       </c>
       <c r="I9" s="5"/>
     </row>
-    <row r="10" spans="1:9" ht="30">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>9</v>
@@ -1051,24 +1314,22 @@
         <v>10</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>26</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>9</v>
@@ -1095,10 +1356,10 @@
         <v>10</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>9</v>
@@ -1112,11 +1373,13 @@
       <c r="H13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I13" s="5"/>
+      <c r="I13" s="5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>10</v>
@@ -1139,28 +1402,26 @@
       <c r="H14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="5" t="s">
-        <v>33</v>
-      </c>
+      <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>9</v>
@@ -1168,26 +1429,28 @@
       <c r="H15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I15" s="5"/>
+      <c r="I15" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>34</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>9</v>
@@ -1233,7 +1496,7 @@
         <v>38</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>9</v>
@@ -1248,62 +1511,62 @@
         <v>10</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>9</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="30">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>10</v>
+        <v>192</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>9</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="30">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>9</v>
@@ -1320,71 +1583,71 @@
         <v>47</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" s="5" t="s">
         <v>48</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I22" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>9</v>
@@ -1398,162 +1661,162 @@
       <c r="H23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I23" s="5" t="s">
-        <v>53</v>
-      </c>
+      <c r="I23" s="5"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I24" s="5"/>
-    </row>
-    <row r="25" spans="1:9" ht="30">
-      <c r="A25" t="s">
+      <c r="B25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I25" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I25" s="1" t="s">
+    </row>
+    <row r="26" spans="1:9" ht="30">
+      <c r="A26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="30">
+      <c r="A27" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" t="s">
-        <v>57</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I26" s="1" t="s">
+      <c r="C27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I27" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
-      <c r="A27" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="30">
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" t="s">
         <v>61</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="30">
-      <c r="A29" t="s">
-        <v>64</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="C29" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>13</v>
@@ -1570,19 +1833,17 @@
       <c r="H29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I29" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="I29" s="5"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>13</v>
@@ -1591,7 +1852,7 @@
         <v>9</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>9</v>
@@ -1603,61 +1864,47 @@
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="I31" s="5"/>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>70</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>9</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
       <c r="I32" s="5"/>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>10</v>
@@ -1672,7 +1919,7 @@
         <v>9</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>9</v>
@@ -1684,10 +1931,10 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>10</v>
@@ -1711,7 +1958,7 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>9</v>
@@ -1729,19 +1976,19 @@
         <v>9</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="I35" s="5"/>
     </row>
-    <row r="36" spans="1:9" ht="30">
+    <row r="36" spans="1:9" ht="45">
       <c r="A36" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>9</v>
@@ -1762,12 +2009,12 @@
         <v>9</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>77</v>
+        <v>197</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>10</v>
@@ -1791,15 +2038,15 @@
         <v>9</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>9</v>
@@ -1820,21 +2067,21 @@
         <v>9</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="30">
       <c r="A39" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>9</v>
+        <v>67</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>10</v>
@@ -1849,15 +2096,15 @@
         <v>9</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="60">
       <c r="A40" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>10</v>
@@ -1878,39 +2125,25 @@
         <v>9</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>87</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I41" s="5"/>
+        <v>190</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>10</v>
@@ -1937,10 +2170,10 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>88</v>
+        <v>191</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>9</v>
@@ -1952,22 +2185,22 @@
         <v>9</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="I43" s="5"/>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>9</v>
@@ -1976,24 +2209,22 @@
         <v>9</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>9</v>
+        <v>195</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I44" s="1" t="s">
-        <v>90</v>
-      </c>
+      <c r="I44" s="5"/>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>10</v>
@@ -2005,25 +2236,27 @@
         <v>9</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I45" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>9</v>
@@ -2032,25 +2265,25 @@
         <v>9</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="I46" s="5"/>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>9</v>
@@ -2065,104 +2298,104 @@
         <v>10</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="I47" s="5"/>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I48" s="1" t="s">
-        <v>95</v>
-      </c>
+      <c r="I48" s="5"/>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>9</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I50" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>9</v>
@@ -2180,18 +2413,16 @@
         <v>9</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>100</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="I51" s="5"/>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>9</v>
@@ -2209,16 +2440,18 @@
         <v>9</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I52" s="5"/>
+        <v>45</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>9</v>
@@ -2233,16 +2466,16 @@
         <v>10</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>85</v>
+        <v>9</v>
       </c>
       <c r="I53" s="5"/>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>10</v>
@@ -2260,21 +2493,19 @@
         <v>10</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>104</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="I54" s="5"/>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>9</v>
@@ -2294,76 +2525,78 @@
       <c r="H55" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I55" s="5"/>
-    </row>
-    <row r="56" spans="1:9" ht="30">
+      <c r="I55" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
       <c r="A56" t="s">
+        <v>99</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I56" s="5"/>
+    </row>
+    <row r="57" spans="1:9" ht="30">
+      <c r="A57" t="s">
+        <v>100</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I57" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I56" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9">
-      <c r="A57" t="s">
-        <v>107</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H57" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I57" s="5"/>
-    </row>
-    <row r="58" spans="1:9" ht="30">
+    </row>
+    <row r="58" spans="1:9">
       <c r="A58" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>10</v>
@@ -2372,104 +2605,104 @@
         <v>10</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>109</v>
+        <v>9</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I58" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9">
+        <v>45</v>
+      </c>
+      <c r="I58" s="5"/>
+    </row>
+    <row r="59" spans="1:9" ht="30">
       <c r="A59" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>10</v>
+        <v>103</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I59" s="5"/>
+        <v>45</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>109</v>
+        <v>10</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I60" s="1" t="s">
-        <v>114</v>
-      </c>
+      <c r="I60" s="5"/>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>9</v>
+        <v>103</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I61" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>9</v>
@@ -2481,7 +2714,7 @@
         <v>9</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>9</v>
@@ -2491,36 +2724,36 @@
       </c>
       <c r="I62" s="5"/>
     </row>
-    <row r="63" spans="1:9" ht="30">
+    <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>118</v>
+        <v>9</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="I63" s="5"/>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" ht="30">
       <c r="A64" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>10</v>
@@ -2532,34 +2765,61 @@
         <v>13</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
-      <c r="H64" s="1"/>
+        <v>112</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="I64" s="5"/>
     </row>
-    <row r="65" spans="2:9">
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
+    <row r="65" spans="1:9">
+      <c r="A65" t="s">
+        <v>113</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
       <c r="I65" s="5"/>
     </row>
-    <row r="66" spans="2:9">
-      <c r="B66" s="1"/>
+    <row r="66" spans="1:9">
+      <c r="A66" t="s">
+        <v>121</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
-      <c r="I66" s="5"/>
-    </row>
-    <row r="67" spans="2:9">
+      <c r="I66" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" t="s">
+        <v>114</v>
+      </c>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
@@ -2567,119 +2827,231 @@
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
-      <c r="I67" s="5"/>
-    </row>
-    <row r="68" spans="2:9">
+      <c r="I67" s="5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" t="s">
+        <v>115</v>
+      </c>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
-      <c r="G68" s="1"/>
-      <c r="H68" s="1"/>
+      <c r="G68" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="I68" s="5"/>
     </row>
-    <row r="69" spans="2:9">
+    <row r="69" spans="1:9">
+      <c r="A69" t="s">
+        <v>116</v>
+      </c>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
+      <c r="E69" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
-      <c r="I69" s="5"/>
-    </row>
-    <row r="70" spans="2:9">
+      <c r="I69" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70" t="s">
+        <v>117</v>
+      </c>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
+      <c r="E70" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
       <c r="I70" s="5"/>
     </row>
-    <row r="71" spans="2:9">
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
+    <row r="71" spans="1:9">
+      <c r="A71" t="s">
+        <v>118</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
+      <c r="E71" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
-      <c r="I71" s="5"/>
-    </row>
-    <row r="72" spans="2:9">
+      <c r="I71" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" t="s">
+        <v>130</v>
+      </c>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
-      <c r="G72" s="1"/>
-      <c r="H72" s="1"/>
+      <c r="F72" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="I72" s="5"/>
     </row>
-    <row r="73" spans="2:9">
+    <row r="73" spans="1:9">
+      <c r="A73" t="s">
+        <v>119</v>
+      </c>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
-      <c r="H73" s="1"/>
-      <c r="I73" s="5"/>
-    </row>
-    <row r="74" spans="2:9">
+      <c r="G73" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I73" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="A74" t="s">
+        <v>128</v>
+      </c>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
-      <c r="G74" s="1"/>
-      <c r="H74" s="1"/>
-      <c r="I74" s="5"/>
-    </row>
-    <row r="75" spans="2:9">
+      <c r="G74" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I74" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75" t="s">
+        <v>120</v>
+      </c>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
-      <c r="H75" s="1"/>
-      <c r="I75" s="5"/>
-    </row>
-    <row r="76" spans="2:9">
-      <c r="B76" s="1"/>
-      <c r="C76" s="1"/>
+      <c r="H75" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I75" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="A76" t="s">
+        <v>122</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
-      <c r="G76" s="1"/>
-      <c r="H76" s="1"/>
-      <c r="I76" s="5"/>
-    </row>
-    <row r="77" spans="2:9">
-      <c r="B77" s="1"/>
-      <c r="C77" s="1"/>
-      <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
-      <c r="F77" s="1"/>
-      <c r="G77" s="1"/>
-      <c r="H77" s="1"/>
-      <c r="I77" s="5"/>
-    </row>
-    <row r="78" spans="2:9">
-      <c r="B78" s="1"/>
-      <c r="C78" s="1"/>
+      <c r="G76" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I76" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="A77" t="s">
+        <v>123</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I77" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
+      <c r="A78" t="s">
+        <v>126</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
-      <c r="G78" s="1"/>
-      <c r="H78" s="1"/>
+      <c r="G78" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="I78" s="5"/>
     </row>
-    <row r="79" spans="2:9">
+    <row r="79" spans="1:9">
+      <c r="A79" t="s">
+        <v>124</v>
+      </c>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
@@ -2689,7 +3061,10 @@
       <c r="H79" s="1"/>
       <c r="I79" s="5"/>
     </row>
-    <row r="80" spans="2:9">
+    <row r="80" spans="1:9">
+      <c r="A80" t="s">
+        <v>125</v>
+      </c>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
@@ -2699,17 +3074,27 @@
       <c r="H80" s="1"/>
       <c r="I80" s="5"/>
     </row>
-    <row r="81" spans="2:9">
+    <row r="81" spans="1:9">
+      <c r="A81" t="s">
+        <v>133</v>
+      </c>
       <c r="B81" s="1"/>
-      <c r="C81" s="1"/>
+      <c r="C81" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
-      <c r="H81" s="1"/>
+      <c r="H81" s="1" t="s">
+        <v>200</v>
+      </c>
       <c r="I81" s="5"/>
     </row>
-    <row r="82" spans="2:9">
+    <row r="82" spans="1:9">
+      <c r="A82" t="s">
+        <v>134</v>
+      </c>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
@@ -2719,7 +3104,10 @@
       <c r="H82" s="1"/>
       <c r="I82" s="5"/>
     </row>
-    <row r="83" spans="2:9">
+    <row r="83" spans="1:9">
+      <c r="A83" t="s">
+        <v>135</v>
+      </c>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
@@ -2729,7 +3117,10 @@
       <c r="H83" s="1"/>
       <c r="I83" s="5"/>
     </row>
-    <row r="84" spans="2:9">
+    <row r="84" spans="1:9">
+      <c r="A84" t="s">
+        <v>136</v>
+      </c>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
@@ -2739,7 +3130,10 @@
       <c r="H84" s="1"/>
       <c r="I84" s="5"/>
     </row>
-    <row r="85" spans="2:9">
+    <row r="85" spans="1:9">
+      <c r="A85" t="s">
+        <v>137</v>
+      </c>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
@@ -2749,7 +3143,10 @@
       <c r="H85" s="1"/>
       <c r="I85" s="5"/>
     </row>
-    <row r="86" spans="2:9">
+    <row r="86" spans="1:9">
+      <c r="A86" t="s">
+        <v>138</v>
+      </c>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
@@ -2759,7 +3156,10 @@
       <c r="H86" s="1"/>
       <c r="I86" s="5"/>
     </row>
-    <row r="87" spans="2:9">
+    <row r="87" spans="1:9">
+      <c r="A87" t="s">
+        <v>139</v>
+      </c>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
@@ -2769,7 +3169,10 @@
       <c r="H87" s="1"/>
       <c r="I87" s="5"/>
     </row>
-    <row r="88" spans="2:9">
+    <row r="88" spans="1:9">
+      <c r="A88" t="s">
+        <v>140</v>
+      </c>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
@@ -2779,7 +3182,10 @@
       <c r="H88" s="1"/>
       <c r="I88" s="5"/>
     </row>
-    <row r="89" spans="2:9">
+    <row r="89" spans="1:9">
+      <c r="A89" t="s">
+        <v>141</v>
+      </c>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
@@ -2787,9 +3193,14 @@
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
       <c r="H89" s="1"/>
-      <c r="I89" s="5"/>
-    </row>
-    <row r="90" spans="2:9">
+      <c r="I89" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9">
+      <c r="A90" t="s">
+        <v>142</v>
+      </c>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
@@ -2799,7 +3210,10 @@
       <c r="H90" s="1"/>
       <c r="I90" s="5"/>
     </row>
-    <row r="91" spans="2:9">
+    <row r="91" spans="1:9">
+      <c r="A91" t="s">
+        <v>143</v>
+      </c>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
@@ -2809,7 +3223,10 @@
       <c r="H91" s="1"/>
       <c r="I91" s="5"/>
     </row>
-    <row r="92" spans="2:9">
+    <row r="92" spans="1:9">
+      <c r="A92" t="s">
+        <v>144</v>
+      </c>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
@@ -2819,7 +3236,10 @@
       <c r="H92" s="1"/>
       <c r="I92" s="5"/>
     </row>
-    <row r="93" spans="2:9">
+    <row r="93" spans="1:9">
+      <c r="A93" t="s">
+        <v>145</v>
+      </c>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
@@ -2829,7 +3249,10 @@
       <c r="H93" s="1"/>
       <c r="I93" s="5"/>
     </row>
-    <row r="94" spans="2:9">
+    <row r="94" spans="1:9">
+      <c r="A94" t="s">
+        <v>146</v>
+      </c>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
@@ -2837,9 +3260,14 @@
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
       <c r="H94" s="1"/>
-      <c r="I94" s="5"/>
-    </row>
-    <row r="95" spans="2:9">
+      <c r="I94" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9">
+      <c r="A95" t="s">
+        <v>147</v>
+      </c>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
@@ -2849,7 +3277,10 @@
       <c r="H95" s="1"/>
       <c r="I95" s="5"/>
     </row>
-    <row r="96" spans="2:9">
+    <row r="96" spans="1:9">
+      <c r="A96" t="s">
+        <v>148</v>
+      </c>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
@@ -2859,17 +3290,29 @@
       <c r="H96" s="1"/>
       <c r="I96" s="5"/>
     </row>
-    <row r="97" spans="2:9">
+    <row r="97" spans="1:9">
+      <c r="A97" t="s">
+        <v>150</v>
+      </c>
       <c r="B97" s="1"/>
-      <c r="C97" s="1"/>
-      <c r="D97" s="1"/>
+      <c r="C97" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
       <c r="G97" s="1"/>
       <c r="H97" s="1"/>
-      <c r="I97" s="5"/>
-    </row>
-    <row r="98" spans="2:9">
+      <c r="I97" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9">
+      <c r="A98" t="s">
+        <v>155</v>
+      </c>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
@@ -2879,17 +3322,37 @@
       <c r="H98" s="1"/>
       <c r="I98" s="5"/>
     </row>
-    <row r="99" spans="2:9">
-      <c r="B99" s="1"/>
-      <c r="C99" s="1"/>
-      <c r="D99" s="1"/>
-      <c r="E99" s="1"/>
-      <c r="F99" s="1"/>
-      <c r="G99" s="1"/>
-      <c r="H99" s="1"/>
+    <row r="99" spans="1:9">
+      <c r="A99" t="s">
+        <v>156</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H99" s="1" t="s">
+        <v>194</v>
+      </c>
       <c r="I99" s="5"/>
     </row>
-    <row r="100" spans="2:9">
+    <row r="100" spans="1:9">
+      <c r="A100" t="s">
+        <v>157</v>
+      </c>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
@@ -2899,7 +3362,10 @@
       <c r="H100" s="1"/>
       <c r="I100" s="5"/>
     </row>
-    <row r="101" spans="2:9">
+    <row r="101" spans="1:9">
+      <c r="A101" t="s">
+        <v>158</v>
+      </c>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
@@ -2909,7 +3375,10 @@
       <c r="H101" s="1"/>
       <c r="I101" s="5"/>
     </row>
-    <row r="102" spans="2:9">
+    <row r="102" spans="1:9">
+      <c r="A102" t="s">
+        <v>159</v>
+      </c>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
@@ -2919,7 +3388,10 @@
       <c r="H102" s="1"/>
       <c r="I102" s="5"/>
     </row>
-    <row r="103" spans="2:9">
+    <row r="103" spans="1:9">
+      <c r="A103" t="s">
+        <v>160</v>
+      </c>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
@@ -2929,7 +3401,10 @@
       <c r="H103" s="1"/>
       <c r="I103" s="5"/>
     </row>
-    <row r="104" spans="2:9">
+    <row r="104" spans="1:9">
+      <c r="A104" t="s">
+        <v>161</v>
+      </c>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
@@ -2939,27 +3414,64 @@
       <c r="H104" s="1"/>
       <c r="I104" s="5"/>
     </row>
-    <row r="105" spans="2:9">
-      <c r="B105" s="1"/>
-      <c r="C105" s="1"/>
-      <c r="D105" s="1"/>
-      <c r="E105" s="1"/>
-      <c r="F105" s="1"/>
-      <c r="G105" s="1"/>
-      <c r="H105" s="1"/>
+    <row r="105" spans="1:9">
+      <c r="A105" t="s">
+        <v>162</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E105" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G105" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H105" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="I105" s="5"/>
     </row>
-    <row r="106" spans="2:9">
-      <c r="B106" s="1"/>
-      <c r="C106" s="1"/>
-      <c r="D106" s="1"/>
-      <c r="E106" s="1"/>
-      <c r="F106" s="1"/>
-      <c r="G106" s="1"/>
-      <c r="H106" s="1"/>
+    <row r="106" spans="1:9">
+      <c r="A106" t="s">
+        <v>163</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H106" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I106" s="5"/>
     </row>
-    <row r="107" spans="2:9">
+    <row r="107" spans="1:9">
+      <c r="A107" t="s">
+        <v>164</v>
+      </c>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
@@ -2967,9 +3479,14 @@
       <c r="F107" s="1"/>
       <c r="G107" s="1"/>
       <c r="H107" s="1"/>
-      <c r="I107" s="5"/>
-    </row>
-    <row r="108" spans="2:9">
+      <c r="I107" s="5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9">
+      <c r="A108" t="s">
+        <v>165</v>
+      </c>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
@@ -2977,9 +3494,14 @@
       <c r="F108" s="1"/>
       <c r="G108" s="1"/>
       <c r="H108" s="1"/>
-      <c r="I108" s="5"/>
-    </row>
-    <row r="109" spans="2:9">
+      <c r="I108" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9">
+      <c r="A109" t="s">
+        <v>168</v>
+      </c>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
@@ -2989,17 +3511,27 @@
       <c r="H109" s="1"/>
       <c r="I109" s="5"/>
     </row>
-    <row r="110" spans="2:9">
+    <row r="110" spans="1:9">
+      <c r="A110" t="s">
+        <v>169</v>
+      </c>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
       <c r="G110" s="1"/>
-      <c r="H110" s="1"/>
-      <c r="I110" s="5"/>
-    </row>
-    <row r="111" spans="2:9">
+      <c r="H110" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="I110" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9">
+      <c r="A111" t="s">
+        <v>171</v>
+      </c>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
@@ -3009,7 +3541,10 @@
       <c r="H111" s="1"/>
       <c r="I111" s="5"/>
     </row>
-    <row r="112" spans="2:9">
+    <row r="112" spans="1:9">
+      <c r="A112" t="s">
+        <v>172</v>
+      </c>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
@@ -3019,7 +3554,10 @@
       <c r="H112" s="1"/>
       <c r="I112" s="5"/>
     </row>
-    <row r="113" spans="2:9">
+    <row r="113" spans="1:9">
+      <c r="A113" t="s">
+        <v>173</v>
+      </c>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
@@ -3029,7 +3567,10 @@
       <c r="H113" s="1"/>
       <c r="I113" s="5"/>
     </row>
-    <row r="114" spans="2:9">
+    <row r="114" spans="1:9">
+      <c r="A114" t="s">
+        <v>174</v>
+      </c>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
@@ -3039,7 +3580,10 @@
       <c r="H114" s="1"/>
       <c r="I114" s="5"/>
     </row>
-    <row r="115" spans="2:9">
+    <row r="115" spans="1:9">
+      <c r="A115" t="s">
+        <v>175</v>
+      </c>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
@@ -3049,7 +3593,10 @@
       <c r="H115" s="1"/>
       <c r="I115" s="5"/>
     </row>
-    <row r="116" spans="2:9">
+    <row r="116" spans="1:9">
+      <c r="A116" t="s">
+        <v>176</v>
+      </c>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
@@ -3059,7 +3606,10 @@
       <c r="H116" s="1"/>
       <c r="I116" s="5"/>
     </row>
-    <row r="117" spans="2:9">
+    <row r="117" spans="1:9">
+      <c r="A117" t="s">
+        <v>184</v>
+      </c>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
@@ -3069,7 +3619,10 @@
       <c r="H117" s="1"/>
       <c r="I117" s="5"/>
     </row>
-    <row r="118" spans="2:9">
+    <row r="118" spans="1:9">
+      <c r="A118" t="s">
+        <v>177</v>
+      </c>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
@@ -3079,7 +3632,10 @@
       <c r="H118" s="1"/>
       <c r="I118" s="5"/>
     </row>
-    <row r="119" spans="2:9">
+    <row r="119" spans="1:9">
+      <c r="A119" t="s">
+        <v>178</v>
+      </c>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
@@ -3089,78 +3645,204 @@
       <c r="H119" s="1"/>
       <c r="I119" s="5"/>
     </row>
-    <row r="120" spans="2:9">
-      <c r="B120" s="1"/>
-      <c r="C120" s="1"/>
-      <c r="D120" s="1"/>
-      <c r="E120" s="1"/>
-      <c r="F120" s="1"/>
-      <c r="G120" s="1"/>
-      <c r="H120" s="1"/>
+    <row r="120" spans="1:9">
+      <c r="A120" t="s">
+        <v>179</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G120" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H120" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I120" s="5"/>
     </row>
-    <row r="121" spans="2:9">
-      <c r="B121" s="1"/>
-      <c r="C121" s="1"/>
-      <c r="D121" s="1"/>
-      <c r="E121" s="1"/>
-      <c r="F121" s="1"/>
-      <c r="G121" s="1"/>
-      <c r="H121" s="1"/>
+    <row r="121" spans="1:9">
+      <c r="A121" t="s">
+        <v>180</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G121" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H121" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="I121" s="5"/>
     </row>
-    <row r="122" spans="2:9">
-      <c r="B122" s="1"/>
-      <c r="C122" s="1"/>
-      <c r="D122" s="1"/>
-      <c r="E122" s="1"/>
-      <c r="F122" s="1"/>
-      <c r="G122" s="1"/>
+    <row r="122" spans="1:9">
+      <c r="A122" t="s">
+        <v>181</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G122" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="H122" s="1"/>
-      <c r="I122" s="5"/>
-    </row>
-    <row r="123" spans="2:9">
-      <c r="B123" s="1"/>
-      <c r="C123" s="1"/>
-      <c r="D123" s="1"/>
-      <c r="E123" s="1"/>
-      <c r="F123" s="1"/>
-      <c r="G123" s="1"/>
-      <c r="H123" s="1"/>
+      <c r="I122" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9">
+      <c r="A123" t="s">
+        <v>182</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G123" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H123" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="I123" s="5"/>
     </row>
-    <row r="124" spans="2:9">
-      <c r="B124" s="1"/>
-      <c r="C124" s="1"/>
-      <c r="D124" s="1"/>
-      <c r="E124" s="1"/>
-      <c r="F124" s="1"/>
-      <c r="G124" s="1"/>
-      <c r="H124" s="1"/>
+    <row r="124" spans="1:9">
+      <c r="A124" t="s">
+        <v>183</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G124" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H124" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="I124" s="5"/>
     </row>
-    <row r="125" spans="2:9">
-      <c r="B125" s="1"/>
-      <c r="C125" s="1"/>
-      <c r="D125" s="1"/>
-      <c r="E125" s="1"/>
-      <c r="F125" s="1"/>
-      <c r="G125" s="1"/>
-      <c r="H125" s="1"/>
+    <row r="125" spans="1:9">
+      <c r="A125" t="s">
+        <v>186</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G125" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H125" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="I125" s="5"/>
     </row>
-    <row r="126" spans="2:9">
-      <c r="B126" s="1"/>
-      <c r="C126" s="1"/>
-      <c r="D126" s="1"/>
-      <c r="E126" s="1"/>
-      <c r="F126" s="1"/>
-      <c r="G126" s="1"/>
-      <c r="H126" s="1"/>
-      <c r="I126" s="5"/>
-    </row>
-    <row r="127" spans="2:9">
-      <c r="B127" s="1"/>
+    <row r="126" spans="1:9">
+      <c r="A126" t="s">
+        <v>187</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G126" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H126" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I126" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9">
+      <c r="A127" t="s">
+        <v>188</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
@@ -3169,7 +3851,7 @@
       <c r="H127" s="1"/>
       <c r="I127" s="5"/>
     </row>
-    <row r="128" spans="2:9">
+    <row r="128" spans="1:9">
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
@@ -3537,6 +4219,7 @@
       <c r="F164" s="1"/>
       <c r="G164" s="1"/>
       <c r="H164" s="1"/>
+      <c r="I164" s="5"/>
     </row>
     <row r="165" spans="2:9">
       <c r="B165" s="1"/>
@@ -3546,6 +4229,7 @@
       <c r="F165" s="1"/>
       <c r="G165" s="1"/>
       <c r="H165" s="1"/>
+      <c r="I165" s="5"/>
     </row>
     <row r="166" spans="2:9">
       <c r="B166" s="1"/>
@@ -3555,6 +4239,7 @@
       <c r="F166" s="1"/>
       <c r="G166" s="1"/>
       <c r="H166" s="1"/>
+      <c r="I166" s="5"/>
     </row>
     <row r="167" spans="2:9">
       <c r="B167" s="1"/>
@@ -3564,13 +4249,65 @@
       <c r="F167" s="1"/>
       <c r="G167" s="1"/>
       <c r="H167" s="1"/>
+      <c r="I167" s="5"/>
+    </row>
+    <row r="168" spans="2:9">
+      <c r="B168" s="1"/>
+      <c r="C168" s="1"/>
+      <c r="D168" s="1"/>
+      <c r="E168" s="1"/>
+      <c r="F168" s="1"/>
+      <c r="G168" s="1"/>
+      <c r="H168" s="1"/>
+      <c r="I168" s="5"/>
+    </row>
+    <row r="169" spans="2:9">
+      <c r="B169" s="1"/>
+      <c r="C169" s="1"/>
+      <c r="D169" s="1"/>
+      <c r="E169" s="1"/>
+      <c r="F169" s="1"/>
+      <c r="G169" s="1"/>
+      <c r="H169" s="1"/>
+    </row>
+    <row r="170" spans="2:9">
+      <c r="B170" s="1"/>
+      <c r="C170" s="1"/>
+      <c r="D170" s="1"/>
+      <c r="E170" s="1"/>
+      <c r="F170" s="1"/>
+      <c r="G170" s="1"/>
+      <c r="H170" s="1"/>
+    </row>
+    <row r="171" spans="2:9">
+      <c r="B171" s="1"/>
+      <c r="C171" s="1"/>
+      <c r="D171" s="1"/>
+      <c r="E171" s="1"/>
+      <c r="F171" s="1"/>
+      <c r="G171" s="1"/>
+      <c r="H171" s="1"/>
+    </row>
+    <row r="172" spans="2:9">
+      <c r="B172" s="1"/>
+      <c r="C172" s="1"/>
+      <c r="D172" s="1"/>
+      <c r="E172" s="1"/>
+      <c r="F172" s="1"/>
+      <c r="G172" s="1"/>
+      <c r="H172" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:J156">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+  <conditionalFormatting sqref="B3:J154">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"?"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3:J161">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -3580,13 +4317,8 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
       <formula>"N"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3:J149">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3596,10 +4328,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3609,12 +4341,18 @@
   <sheetData>
     <row r="1" spans="1:1" ht="105">
       <c r="A1" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="270">
-      <c r="A3" s="1" t="s">
-        <v>69</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1"/>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="5" spans="1:1" ht="270">
+      <c r="A5" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Roy's terrible sadistic castle B started
</commit_message>
<xml_diff>
--- a/OverworldRouting.xlsx
+++ b/OverworldRouting.xlsx
@@ -1038,8 +1038,8 @@
   <dimension ref="A1:I172"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I68" sqref="I68"/>
+      <pane ySplit="2" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>